<commit_message>
Bootstrap metrics/SOTA models added
</commit_message>
<xml_diff>
--- a/benchmark/b_imputation.xlsx
+++ b/benchmark/b_imputation.xlsx
@@ -542,49 +542,49 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9597646895015316</v>
+        <v>0.959175717070454</v>
       </c>
       <c r="C2" t="n">
-        <v>0.89736355226642</v>
+        <v>0.899444958371878</v>
       </c>
       <c r="D2" t="n">
         <v>0.8923684210526316</v>
       </c>
       <c r="E2" t="n">
-        <v>0.868155929038282</v>
+        <v>0.8706204236080397</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9011904761904761</v>
+        <v>0.9047619047619048</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9242351199247751</v>
+        <v>0.9242656449553002</v>
       </c>
       <c r="H2" t="n">
-        <v>0.02104349861719232</v>
+        <v>0.02151508790621114</v>
       </c>
       <c r="I2" t="n">
-        <v>0.04010676322158118</v>
+        <v>0.03806435376428949</v>
       </c>
       <c r="J2" t="n">
         <v>0.08221736611482228</v>
       </c>
       <c r="K2" t="n">
-        <v>0.04947898540426823</v>
+        <v>0.03673459897686258</v>
       </c>
       <c r="L2" t="n">
-        <v>0.04537827533831511</v>
+        <v>0.03072531109379957</v>
       </c>
       <c r="M2" t="n">
-        <v>0.05652883947865767</v>
+        <v>0.05647417221222185</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>[0.945, 0.975]</t>
+          <t>[0.944, 0.975]</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>[0.869, 0.926]</t>
+          <t>[0.872, 0.927]</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -594,12 +594,12 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>[0.833, 0.904]</t>
+          <t>[0.844, 0.897]</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>[0.869, 0.934]</t>
+          <t>[0.883, 0.927]</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="T3" t="n">
-        <v>0.09422893327591718</v>
+        <v>0.06862723695369878</v>
       </c>
     </row>
     <row r="4">
@@ -758,7 +758,7 @@
         </is>
       </c>
       <c r="T4" t="n">
-        <v>0.1631507604774231</v>
+        <v>0.1366846762177055</v>
       </c>
     </row>
     <row r="5">
@@ -834,7 +834,7 @@
         </is>
       </c>
       <c r="T5" t="n">
-        <v>0.2631138617210181</v>
+        <v>0.3674628466525119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>